<commit_message>
Update Effortlog and WeeklyReport
</commit_message>
<xml_diff>
--- a/1.DELIVERABLE/1.10 EFFORT_LOG/Week21/BSS_EffortLog_HaiTran_Week21.xlsx
+++ b/1.DELIVERABLE/1.10 EFFORT_LOG/Week21/BSS_EffortLog_HaiTran_Week21.xlsx
@@ -51,37 +51,37 @@
     <t>Training Technical</t>
   </si>
   <si>
-    <t>Implement "Create draft" function</t>
+    <t>WEEK: 21</t>
   </si>
   <si>
-    <t>13/2/2017</t>
+    <t>Implement "View News" function on server</t>
   </si>
   <si>
-    <t>Demo "View News" function</t>
+    <t>Implement "View News" function on frontend for user</t>
   </si>
   <si>
-    <t>14/2/2017</t>
+    <t>Implement "Transfer News" function on frontend</t>
   </si>
   <si>
-    <t>Demo "Create Draft" function</t>
+    <t>Implement "Edit News"function on frontend</t>
   </si>
   <si>
-    <t>Demo "Edit News" function</t>
+    <t>Presentation EOMP2</t>
   </si>
   <si>
-    <t>15/2/2017</t>
+    <t>20/2/2017</t>
   </si>
   <si>
-    <t>Implement "Sort News" function</t>
+    <t>23/2/2017</t>
   </si>
   <si>
-    <t>16/2/2017</t>
+    <t>24/2/2017</t>
   </si>
   <si>
-    <t>18/2/2017</t>
+    <t>25/2/2017</t>
   </si>
   <si>
-    <t>WEEK: 20</t>
+    <t>22/2/2017</t>
   </si>
 </sst>
 </file>
@@ -211,13 +211,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,7 +524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -535,7 +535,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,14 +553,14 @@
     <row r="1" spans="1:27" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -584,14 +584,14 @@
     <row r="2" spans="1:27" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="12" t="s">
-        <v>20</v>
+      <c r="C2" s="13" t="s">
+        <v>10</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -688,20 +688,20 @@
       <c r="C5" s="10">
         <v>1</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>7</v>
+      <c r="D5" s="11" t="s">
+        <v>11</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G5" s="9">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H5" s="9">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -729,20 +729,20 @@
       <c r="C6" s="10">
         <v>2</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>10</v>
+      <c r="D6" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G6" s="9">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H6" s="9">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -770,14 +770,14 @@
       <c r="C7" s="10">
         <v>3</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>12</v>
+      <c r="D7" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G7" s="9">
         <v>2</v>
@@ -811,20 +811,20 @@
       <c r="C8" s="10">
         <v>4</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>9</v>
+      <c r="D8" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G8" s="9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H8" s="9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -852,20 +852,20 @@
       <c r="C9" s="10">
         <v>5</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G9" s="9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H9" s="9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -893,17 +893,17 @@
       <c r="C10" s="10">
         <v>6</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>15</v>
+      <c r="D10" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G10" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="9">
         <v>3</v>
@@ -934,20 +934,20 @@
       <c r="C11" s="10">
         <v>7</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>8</v>
+      <c r="D11" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G11" s="9">
         <v>2</v>
       </c>
       <c r="H11" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -975,20 +975,20 @@
       <c r="C12" s="10">
         <v>8</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>17</v>
+      <c r="D12" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>19</v>
       </c>
       <c r="G12" s="9">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="H12" s="9">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>

</xml_diff>